<commit_message>
improving and bug fixe
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -12,9 +12,10 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="26895" windowHeight="9900"/>
   </bookViews>
   <sheets>
-    <sheet name="diag_max-Uniform" sheetId="4" r:id="rId1"/>
-    <sheet name="diag_max-Binomial a=4 b=0.5" sheetId="1" r:id="rId2"/>
-    <sheet name="shuffle-Uniform" sheetId="2" r:id="rId3"/>
+    <sheet name="why k=n-1" sheetId="5" r:id="rId1"/>
+    <sheet name="diag_max-Uniform" sheetId="4" r:id="rId2"/>
+    <sheet name="diag_max-Binomial a=4 b=0.5" sheetId="1" r:id="rId3"/>
+    <sheet name="shuffle-Uniform" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -248,7 +249,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="132">
   <si>
     <t>Uniform</t>
   </si>
@@ -632,13 +633,28 @@
   </si>
   <si>
     <t>100x100_4_0.5</t>
+  </si>
+  <si>
+    <t>('icNO', '1iF1')</t>
+  </si>
+  <si>
+    <t>('hefO', 'L6LC')</t>
+  </si>
+  <si>
+    <t>k/n</t>
+  </si>
+  <si>
+    <t>('R8Ay', 'PAUa')</t>
+  </si>
+  <si>
+    <t>Time [s]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -647,8 +663,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -667,20 +684,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="4" tint="-0.499984740745262"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="9" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
@@ -692,6 +695,30 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="4" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -714,7 +741,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -723,12 +750,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -740,16 +761,26 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1031,16 +1062,549 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" style="2" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1" s="8">
+        <v>3</v>
+      </c>
+      <c r="C1" s="8">
+        <v>4</v>
+      </c>
+      <c r="D1" s="8">
+        <v>5</v>
+      </c>
+      <c r="E1" s="8">
+        <v>6</v>
+      </c>
+      <c r="F1" s="8">
+        <v>7</v>
+      </c>
+      <c r="G1" s="8">
+        <v>8</v>
+      </c>
+      <c r="H1" s="8">
+        <v>9</v>
+      </c>
+      <c r="I1" s="8">
+        <v>10</v>
+      </c>
+      <c r="J1" s="8">
+        <v>11</v>
+      </c>
+      <c r="K1" s="8">
+        <v>12</v>
+      </c>
+      <c r="L1" s="8">
+        <v>13</v>
+      </c>
+      <c r="M1" s="8">
+        <v>14</v>
+      </c>
+      <c r="N1" s="8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.46500000000000002</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.8911</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.89019999999999999</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.90029999999999999</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1.0478000000000001</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1.1119000000000001</v>
+      </c>
+      <c r="H2" s="2">
+        <v>1.1015999999999999</v>
+      </c>
+      <c r="I2" s="2">
+        <v>1.0570999999999999</v>
+      </c>
+      <c r="J2" s="2">
+        <v>1.1444000000000001</v>
+      </c>
+      <c r="K2" s="2">
+        <v>1.0176000000000001</v>
+      </c>
+      <c r="L2" s="2">
+        <v>1.0868</v>
+      </c>
+      <c r="M2" s="2">
+        <v>1.0739000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>9.2700000000000005E-2</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.44969999999999999</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.5242</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.55910000000000004</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.70279999999999998</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0.75880000000000003</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0.78869999999999996</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0.77969999999999995</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0.8619</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0.78500000000000003</v>
+      </c>
+      <c r="L3" s="2">
+        <v>0.84060000000000001</v>
+      </c>
+      <c r="M3" s="2">
+        <v>0.84640000000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2">
+        <v>0.16789999999999999</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.30080000000000001</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.36180000000000001</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.46989999999999998</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.52300000000000002</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0.60140000000000005</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0.59540000000000004</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0.66769999999999996</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0.63480000000000003</v>
+      </c>
+      <c r="L4" s="2">
+        <v>0.67979999999999996</v>
+      </c>
+      <c r="M4" s="2">
+        <v>0.69230000000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2">
+        <v>0.14030000000000001</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.31900000000000001</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0.36420000000000002</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.44090000000000001</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0.46960000000000002</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0.52729999999999999</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0.51529999999999998</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0.55259999999999998</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0.57430000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2">
+        <v>8.2900000000000001E-2</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.1792</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.23899999999999999</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.33839999999999998</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0.35959999999999998</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0.42420000000000002</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0.4214</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0.4556</v>
+      </c>
+      <c r="M6" s="2">
+        <v>0.4345</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2">
+        <v>7.3200000000000001E-2</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0.14940000000000001</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0.2392</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0.26490000000000002</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0.33179999999999998</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0.34079999999999999</v>
+      </c>
+      <c r="L7" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="M7" s="2">
+        <v>0.35670000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2">
+        <v>6.9400000000000003E-2</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0.14829999999999999</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0.1862</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0.24859999999999999</v>
+      </c>
+      <c r="K8" s="2">
+        <v>0.51529999999999998</v>
+      </c>
+      <c r="L8" s="2">
+        <v>0.30459999999999998</v>
+      </c>
+      <c r="M8" s="2">
+        <v>0.30109999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2">
+        <v>6.2199999999999998E-2</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0.1111</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0.1812</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0.2135</v>
+      </c>
+      <c r="L9" s="2">
+        <v>0.2399</v>
+      </c>
+      <c r="M9" s="2">
+        <v>0.27610000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2">
+        <v>5.2400000000000002E-2</v>
+      </c>
+      <c r="J10" s="2">
+        <v>0.1168</v>
+      </c>
+      <c r="K10" s="2">
+        <v>0.1555</v>
+      </c>
+      <c r="L10" s="2">
+        <v>0.18559999999999999</v>
+      </c>
+      <c r="M10" s="2">
+        <v>0.22900000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2">
+        <v>5.8299999999999998E-2</v>
+      </c>
+      <c r="K11" s="2">
+        <v>9.6500000000000002E-2</v>
+      </c>
+      <c r="L11" s="2">
+        <v>0.13650000000000001</v>
+      </c>
+      <c r="M11" s="2">
+        <v>0.1731</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2">
+        <v>4.6600000000000003E-2</v>
+      </c>
+      <c r="L12" s="2">
+        <v>8.8599999999999998E-2</v>
+      </c>
+      <c r="M12" s="2">
+        <v>0.12740000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2">
+        <v>4.3499999999999997E-2</v>
+      </c>
+      <c r="M13" s="2">
+        <v>8.1799999999999998E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2">
+        <v>3.9600000000000003E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B17">
+        <v>1.0987</v>
+      </c>
+      <c r="C17">
+        <v>1.1106</v>
+      </c>
+      <c r="D17">
+        <v>1.0814999999999999</v>
+      </c>
+      <c r="E17">
+        <v>1.1545000000000001</v>
+      </c>
+      <c r="F17">
+        <v>1.4650000000000001</v>
+      </c>
+      <c r="G17">
+        <v>3.2953000000000001</v>
+      </c>
+      <c r="H17">
+        <v>14.9739</v>
+      </c>
+      <c r="I17">
+        <v>93.9876</v>
+      </c>
+      <c r="J17">
+        <v>707.23</v>
+      </c>
+      <c r="K17">
+        <v>4746.9807000000001</v>
+      </c>
+      <c r="L17">
+        <v>35588.241699999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.5703125" style="2" bestFit="1" customWidth="1"/>
@@ -1053,43 +1617,43 @@
     <col min="11" max="11" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:11" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="12" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="8" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="2">
@@ -1125,7 +1689,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="8" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1157,7 +1721,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1189,7 +1753,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="8" t="s">
         <v>20</v>
       </c>
       <c r="B5" s="2">
@@ -1225,7 +1789,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="8" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -1257,7 +1821,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -1289,7 +1853,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="8" t="s">
         <v>29</v>
       </c>
       <c r="B8" s="2">
@@ -1325,7 +1889,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="8" t="s">
         <v>30</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -1357,7 +1921,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="8" t="s">
         <v>31</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -1389,13 +1953,13 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="8" t="s">
         <v>37</v>
       </c>
       <c r="B11" s="2">
         <v>198</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="5">
         <v>13</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -1425,7 +1989,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="8" t="s">
         <v>40</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1457,7 +2021,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="8" t="s">
         <v>41</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -1489,7 +2053,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="8" t="s">
         <v>42</v>
       </c>
       <c r="B14" s="2">
@@ -1525,7 +2089,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="8" t="s">
         <v>38</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -1557,7 +2121,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="8" t="s">
         <v>43</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -1589,7 +2153,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="8" t="s">
         <v>44</v>
       </c>
       <c r="B17" s="2">
@@ -1625,7 +2189,7 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="8" t="s">
         <v>45</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1657,7 +2221,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="8" t="s">
         <v>39</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -1689,7 +2253,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="8" t="s">
         <v>46</v>
       </c>
       <c r="B20" s="2">
@@ -1725,7 +2289,7 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="8" t="s">
         <v>47</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -1757,7 +2321,7 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="8" t="s">
         <v>48</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -1789,7 +2353,7 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B23" s="2">
@@ -1825,7 +2389,7 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -1857,7 +2421,7 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -1889,13 +2453,13 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B26" s="4">
         <v>1380000000</v>
       </c>
-      <c r="C26" s="8">
+      <c r="C26" s="6">
         <v>99</v>
       </c>
       <c r="D26" s="2" t="s">
@@ -1922,13 +2486,13 @@
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="8" t="s">
         <v>86</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="4" t="s">
         <v>95</v>
       </c>
       <c r="D27" s="2" t="s">
@@ -1951,13 +2515,13 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="8" t="s">
         <v>87</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="4" t="s">
         <v>95</v>
       </c>
       <c r="D28" s="2" t="s">
@@ -1980,13 +2544,13 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="6">
+      <c r="B29" s="4">
         <v>51700000000000</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C29" s="5">
         <v>181</v>
       </c>
       <c r="D29" s="2" t="s">
@@ -2010,13 +2574,13 @@
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="6">
+      <c r="B30" s="4">
         <v>8.4699999999999994E+23</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="5">
         <v>422</v>
       </c>
       <c r="D30" s="2" t="s">
@@ -2040,13 +2604,13 @@
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B31" s="6">
+      <c r="B31" s="4">
         <v>1.57E+35</v>
       </c>
-      <c r="C31" s="7">
+      <c r="C31" s="5">
         <v>762</v>
       </c>
       <c r="D31" s="2" t="s">
@@ -2070,10 +2634,10 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B32" s="6">
+      <c r="B32" s="4">
         <v>1.86E+47</v>
       </c>
       <c r="C32" s="2">
@@ -2100,10 +2664,10 @@
       </c>
     </row>
     <row r="33" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="B33" s="6">
+      <c r="B33" s="4">
         <v>9.7699999999999998E+59</v>
       </c>
       <c r="C33" s="2">
@@ -2130,58 +2694,100 @@
       </c>
     </row>
     <row r="34" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="B34" s="6">
+      <c r="B34" s="4">
         <v>1.8099999999999999E+73</v>
       </c>
       <c r="C34" s="2">
         <v>2380</v>
       </c>
-      <c r="J34" s="1"/>
+      <c r="D34" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="G34" s="2">
+        <v>312.50459999999998</v>
+      </c>
+      <c r="H34" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="I34" s="2">
+        <v>1508</v>
+      </c>
+      <c r="J34" s="1">
+        <v>6.5092999999999996</v>
+      </c>
       <c r="K34" s="2">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>36.638655462184879</v>
       </c>
     </row>
     <row r="35" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="B35" s="6">
+      <c r="B35" s="4">
         <v>9.91E+86</v>
       </c>
       <c r="C35" s="2">
         <v>3120</v>
       </c>
-      <c r="J35" s="1"/>
+      <c r="D35" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="G35" s="2">
+        <v>551.07989999999995</v>
+      </c>
+      <c r="H35" s="2">
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="I35" s="2">
+        <v>2049</v>
+      </c>
+      <c r="J35" s="1">
+        <v>9.0724</v>
+      </c>
       <c r="K35" s="2">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>34.32692307692308</v>
       </c>
     </row>
     <row r="36" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="B36" s="6">
+      <c r="B36" s="4">
         <v>1.4200000000000001E+101</v>
       </c>
       <c r="C36" s="2">
         <v>3960</v>
       </c>
-      <c r="J36" s="1"/>
+      <c r="D36" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="G36" s="2">
+        <v>883.87260000000003</v>
+      </c>
+      <c r="H36" s="2">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="I36" s="2">
+        <v>2628</v>
+      </c>
+      <c r="J36" s="1">
+        <v>13.0036</v>
+      </c>
       <c r="K36" s="2">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>33.636363636363633</v>
       </c>
     </row>
     <row r="37" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B37" s="6">
+      <c r="B37" s="4">
         <v>4.7600000000000001E+115</v>
       </c>
       <c r="C37" s="2">
@@ -2213,17 +2819,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.5703125" style="2" bestFit="1" customWidth="1"/>
@@ -2236,43 +2842,43 @@
     <col min="11" max="11" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:11" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="14" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="8" t="s">
         <v>109</v>
       </c>
       <c r="B2" s="2">
@@ -2289,7 +2895,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="8" t="s">
         <v>110</v>
       </c>
       <c r="B3" s="2">
@@ -2305,7 +2911,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="8" t="s">
         <v>111</v>
       </c>
       <c r="B4" s="2">
@@ -2322,13 +2928,13 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="8" t="s">
         <v>112</v>
       </c>
       <c r="B5" s="2">
         <v>198</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="5">
         <v>13</v>
       </c>
       <c r="E5" s="3"/>
@@ -2338,7 +2944,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="8" t="s">
         <v>113</v>
       </c>
       <c r="B6" s="2">
@@ -2350,7 +2956,7 @@
       <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="8" t="s">
         <v>114</v>
       </c>
       <c r="B7" s="2">
@@ -2366,7 +2972,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="8" t="s">
         <v>115</v>
       </c>
       <c r="B8" s="2">
@@ -2382,7 +2988,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="8" t="s">
         <v>116</v>
       </c>
       <c r="B9" s="2">
@@ -2394,25 +3000,25 @@
       <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="4">
         <v>1380000000</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="5">
         <v>99</v>
       </c>
       <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="4">
         <v>51700000000000</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="5">
         <v>181</v>
       </c>
       <c r="K11" s="1">
@@ -2421,13 +3027,13 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="4">
         <v>8.4699999999999994E+23</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="5">
         <v>422</v>
       </c>
       <c r="K12" s="1">
@@ -2436,13 +3042,13 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="4">
         <v>1.57E+35</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="5">
         <v>762</v>
       </c>
       <c r="K13" s="1">
@@ -2451,10 +3057,10 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="4">
         <v>1.86E+47</v>
       </c>
       <c r="C14" s="2">
@@ -2466,10 +3072,10 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="4">
         <v>9.7699999999999998E+59</v>
       </c>
       <c r="C15" s="2">
@@ -2481,10 +3087,10 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="4">
         <v>1.8099999999999999E+73</v>
       </c>
       <c r="C16" s="2">
@@ -2496,10 +3102,10 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="4">
         <v>9.91E+86</v>
       </c>
       <c r="C17" s="2">
@@ -2511,10 +3117,10 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="4">
         <v>1.4200000000000001E+101</v>
       </c>
       <c r="C18" s="2">
@@ -2526,10 +3132,10 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="4">
         <v>4.7600000000000001E+115</v>
       </c>
       <c r="C19" s="2">
@@ -2546,17 +3152,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.5703125" style="2" bestFit="1" customWidth="1"/>
@@ -2568,44 +3174,44 @@
     <col min="10" max="10" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:12" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4"/>
-      <c r="L1" s="10" t="s">
+      <c r="K1" s="7"/>
+      <c r="L1" s="9" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="8" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="2">
@@ -2618,7 +3224,7 @@
       <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="8" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -2630,7 +3236,7 @@
       <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -2642,7 +3248,7 @@
       <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="8" t="s">
         <v>20</v>
       </c>
       <c r="B5" s="2">
@@ -2654,7 +3260,7 @@
       <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="8" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -2666,7 +3272,7 @@
       <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -2678,7 +3284,7 @@
       <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="8" t="s">
         <v>29</v>
       </c>
       <c r="B8" s="2">
@@ -2691,7 +3297,7 @@
       <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="8" t="s">
         <v>30</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -2704,7 +3310,7 @@
       <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="8" t="s">
         <v>31</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -2716,19 +3322,19 @@
       <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="8" t="s">
         <v>37</v>
       </c>
       <c r="B11" s="2">
         <v>198</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="5">
         <v>13</v>
       </c>
       <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="8" t="s">
         <v>40</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -2740,7 +3346,7 @@
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="8" t="s">
         <v>41</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -2752,7 +3358,7 @@
       <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="8" t="s">
         <v>42</v>
       </c>
       <c r="B14" s="2">
@@ -2764,7 +3370,7 @@
       <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="8" t="s">
         <v>38</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -2776,7 +3382,7 @@
       <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="8" t="s">
         <v>43</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -2788,7 +3394,7 @@
       <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="8" t="s">
         <v>44</v>
       </c>
       <c r="B17" s="2">
@@ -2800,7 +3406,7 @@
       <c r="E17" s="3"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="8" t="s">
         <v>45</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -2812,7 +3418,7 @@
       <c r="E18" s="3"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="8" t="s">
         <v>39</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -2824,7 +3430,7 @@
       <c r="E19" s="3"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="8" t="s">
         <v>46</v>
       </c>
       <c r="B20" s="2">
@@ -2836,7 +3442,7 @@
       <c r="E20" s="3"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="8" t="s">
         <v>47</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -2848,7 +3454,7 @@
       <c r="E21" s="3"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="8" t="s">
         <v>48</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -2860,7 +3466,7 @@
       <c r="E22" s="3"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B23" s="2">
@@ -2871,7 +3477,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -2883,7 +3489,7 @@
       <c r="E24" s="3"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -2895,79 +3501,79 @@
       <c r="E25" s="3"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B26" s="4">
         <v>1380000000</v>
       </c>
-      <c r="C26" s="8">
+      <c r="C26" s="6">
         <v>99</v>
       </c>
       <c r="E26" s="3"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="8" t="s">
         <v>86</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="4" t="s">
         <v>95</v>
       </c>
       <c r="E27" s="3"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="8" t="s">
         <v>87</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="4" t="s">
         <v>95</v>
       </c>
       <c r="E28" s="3"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="6">
+      <c r="B29" s="4">
         <v>51700000000000</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C29" s="5">
         <v>181</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="6">
+      <c r="B30" s="4">
         <v>8.4699999999999994E+23</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="5">
         <v>422</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B31" s="6">
+      <c r="B31" s="4">
         <v>1.57E+35</v>
       </c>
-      <c r="C31" s="7">
+      <c r="C31" s="5">
         <v>762</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B32" s="6">
+      <c r="B32" s="4">
         <v>1.86E+47</v>
       </c>
       <c r="C32" s="2">
@@ -2975,10 +3581,10 @@
       </c>
     </row>
     <row r="33" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="B33" s="6">
+      <c r="B33" s="4">
         <v>9.7699999999999998E+59</v>
       </c>
       <c r="C33" s="2">
@@ -2987,10 +3593,10 @@
       <c r="J33" s="1"/>
     </row>
     <row r="34" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="B34" s="6">
+      <c r="B34" s="4">
         <v>1.8099999999999999E+73</v>
       </c>
       <c r="C34" s="2">
@@ -2999,10 +3605,10 @@
       <c r="J34" s="1"/>
     </row>
     <row r="35" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="B35" s="6">
+      <c r="B35" s="4">
         <v>9.91E+86</v>
       </c>
       <c r="C35" s="2">
@@ -3011,10 +3617,10 @@
       <c r="J35" s="1"/>
     </row>
     <row r="36" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="B36" s="6">
+      <c r="B36" s="4">
         <v>1.4200000000000001E+101</v>
       </c>
       <c r="C36" s="2">
@@ -3023,10 +3629,10 @@
       <c r="J36" s="1"/>
     </row>
     <row r="37" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B37" s="6">
+      <c r="B37" s="4">
         <v>4.7600000000000001E+115</v>
       </c>
       <c r="C37" s="2">

</xml_diff>